<commit_message>
added grafik lansia chart target 2023
</commit_message>
<xml_diff>
--- a/excel/LANSIA2022.xlsx
+++ b/excel/LANSIA2022.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminz\Desktop\reportigdpetir\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7995E220-BCE9-4763-B4E6-729654215385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E7F10E-B026-42F1-8161-3A5FBB380C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="825" windowWidth="21600" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1095" windowWidth="10755" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LANSIA2022" sheetId="1" r:id="rId1"/>
-    <sheet name="2023" sheetId="2" r:id="rId2"/>
+    <sheet name="TARGET2023" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Bulan</t>
   </si>
@@ -78,15 +78,6 @@
     <t>desember</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>BPJS</t>
-  </si>
-  <si>
-    <t>Umum</t>
-  </si>
-  <si>
     <t>Pra Lansia</t>
   </si>
   <si>
@@ -94,13 +85,37 @@
   </si>
   <si>
     <t>Lansia Risti</t>
+  </si>
+  <si>
+    <t>45-49 tahun</t>
+  </si>
+  <si>
+    <t>50-54 tahun</t>
+  </si>
+  <si>
+    <t>55-59 tahun</t>
+  </si>
+  <si>
+    <t>60-64 tahun</t>
+  </si>
+  <si>
+    <t>65-69 tahun</t>
+  </si>
+  <si>
+    <t>&gt; 70 tahun</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>umur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +123,11 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,15 +156,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{CA26F9BD-F968-4CCB-B16C-4446B7A153F1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -469,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -653,134 +675,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D528824F-2A2D-4421-BE3D-F6883A8E2959}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D13" si="0">SUM(B2:C2)</f>
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>786</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>